<commit_message>
corrected location table data constraint.
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/loc_hierarchy_list.xlsx
+++ b/mosip_master/xlsx/loc_hierarchy_list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rakshitha.M\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Develop_Branch_all\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$19</definedName>
+  </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -443,7 +446,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,7 +534,7 @@
       <c r="B6" s="5">
         <v>1</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -721,6 +724,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D19"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>